<commit_message>
Updated to add tag
</commit_message>
<xml_diff>
--- a/Indigency-Test-v2.xlsx
+++ b/Indigency-Test-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sandbox\repo\karappatan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17339F5E-4E94-41DB-BE41-9828AC887849}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459110F5-5F72-402E-A7F4-03F290F5C65C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="33749" windowHeight="18183" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="33749" windowHeight="18183" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Module" sheetId="1" r:id="rId1"/>
@@ -1237,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1629,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CADE153-7C56-4286-AE0A-C29964A6ABC9}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>

</xml_diff>